<commit_message>
Added the link to the Medium article that describes the risk management approach.
</commit_message>
<xml_diff>
--- a/Risk Log.xlsx
+++ b/Risk Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\risk-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4D6704-D3A3-4FFA-9540-5AAA2CF2A34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721C4A93-D103-4ADC-A8CC-7ED2CE005D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2087,6 +2087,60 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2124,8 +2178,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2136,13 +2188,23 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="hair">
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
           <color auto="1"/>
         </left>
         <right/>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2166,11 +2228,25 @@
         <left style="hair">
           <color auto="1"/>
         </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
         <right style="hair">
           <color auto="1"/>
         </right>
         <top/>
         <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2202,6 +2278,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2230,6 +2322,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2258,6 +2366,23 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2286,6 +2411,23 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2314,6 +2456,23 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2342,6 +2501,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2370,6 +2545,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2398,6 +2589,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2426,6 +2633,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2454,6 +2677,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2482,6 +2721,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2510,6 +2765,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2538,6 +2809,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2555,12 +2842,30 @@
         <scheme val="none"/>
       </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
         <right style="hair">
           <color auto="1"/>
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2582,7 +2887,7 @@
       </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
-        <right style="thick">
+        <right style="hair">
           <color auto="1"/>
         </right>
         <top/>
@@ -2590,64 +2895,28 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="hair">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2658,282 +2927,13 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thick">
           <color auto="1"/>
         </right>
         <top/>
         <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="hair">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -5446,7 +5446,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> (https://github.com/bks07/risk-log) and write a Medium article to share it with others. You can find the article "Easy Risk Management with Jira" at ... There, you can find everything you need to work with this file.</a:t>
+            <a:t> (https://github.com/bks07/risk-log) and write a Medium article to share it with others. You can find the article "Easy Risk Management with Jira, Confluence, and Excel" at https://medium.com/agileinsider/easy-risk-management-with-jira-confluence-and-excel-c7b2dd13f848. There, you can find everything you need to work with this file.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0">
             <a:solidFill>
@@ -5833,24 +5833,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="EXP_Risks" displayName="EXP_Risks" ref="A1:R3" totalsRowCount="1" headerRowDxfId="83" totalsRowDxfId="81" tableBorderDxfId="82">
   <autoFilter ref="A1:R2" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="issueKey" dataDxfId="80" totalsRowDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{AD6A686B-8F8B-4FBE-B181-B817BB14804F}" name="issueID" dataDxfId="79" totalsRowDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{9CC9F1D9-CD69-4790-A219-2EFAA2BFCA2D}" name="issueType" dataDxfId="78" totalsRowDxfId="42"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Reporter" dataDxfId="77" totalsRowDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{66525FB4-7D9E-4BDB-8167-3CE5128D4A64}" name="Reporter ID" dataDxfId="76" totalsRowDxfId="40"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Assignee" dataDxfId="75" totalsRowDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{F3D52168-82EC-47B5-8E46-99B870FCF857}" name="Assignee ID" dataDxfId="74" totalsRowDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Summary" dataDxfId="73" totalsRowDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Status" dataDxfId="72" totalsRowDxfId="36"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="Resolution" dataDxfId="71" totalsRowDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{2CE72620-5AA0-409F-9521-C74F80C796B3}" name="Priority" dataDxfId="70" totalsRowDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="Created" dataDxfId="69" totalsRowDxfId="33"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Resolved" dataDxfId="68" totalsRowDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{EA48B66D-5068-4E9E-80EA-183BE54B7FB5}" name="Flagged" dataDxfId="67" totalsRowDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{B8D55795-6D07-42AC-AB88-61EC4671F14F}" name="Labels" dataDxfId="66" totalsRowDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="field::impact" dataDxfId="65" totalsRowDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="field::likelihood" dataDxfId="64" totalsRowDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="BL.existsInRiskLog" dataDxfId="63" totalsRowDxfId="27">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="issueKey" dataDxfId="80" totalsRowDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{AD6A686B-8F8B-4FBE-B181-B817BB14804F}" name="issueID" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{9CC9F1D9-CD69-4790-A219-2EFAA2BFCA2D}" name="issueType" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0200-000015000000}" name="Reporter" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="10" xr3:uid="{66525FB4-7D9E-4BDB-8167-3CE5128D4A64}" name="Reporter ID" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0200-000014000000}" name="Assignee" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{F3D52168-82EC-47B5-8E46-99B870FCF857}" name="Assignee ID" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Summary" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Status" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0200-000017000000}" name="Resolution" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{2CE72620-5AA0-409F-9521-C74F80C796B3}" name="Priority" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0200-000018000000}" name="Created" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0200-000016000000}" name="Resolved" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{EA48B66D-5068-4E9E-80EA-183BE54B7FB5}" name="Flagged" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="13" xr3:uid="{B8D55795-6D07-42AC-AB88-61EC4671F14F}" name="Labels" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="field::impact" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="field::likelihood" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="BL.existsInRiskLog" dataDxfId="46" totalsRowDxfId="45">
       <calculatedColumnFormula>IF(EXP_Risks[[#This Row],[issueKey]]&lt;&gt;"",COUNTIF(TBL_RiskLog[Key],EXP_Risks[[#This Row],[issueKey]]),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5859,36 +5859,36 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="MD_Impact" displayName="MD_Impact" ref="A11:C17" totalsRowShown="0" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="MD_Impact" displayName="MD_Impact" ref="A11:C17" totalsRowShown="0" dataDxfId="44">
   <autoFilter ref="A11:C17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Name" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Order" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Description" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Name" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Order" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Description" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="MD_Likelihood" displayName="MD_Likelihood" ref="A2:C8" totalsRowShown="0" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="MD_Likelihood" displayName="MD_Likelihood" ref="A2:C8" totalsRowShown="0" dataDxfId="40">
   <autoFilter ref="A2:C8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Name" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Order" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Description" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Name" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Order" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Description" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="MD_RiskStrategies" displayName="MD_RiskStrategies" ref="A52:C56" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="MD_RiskStrategies" displayName="MD_RiskStrategies" ref="A52:C56" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="A52:C56" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Name" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Order" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Name" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Order" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Description" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5910,18 +5910,18 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="MD_SeverityMapping" displayName="MD_SeverityMapping" ref="A59:D95" totalsRowShown="0" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="MD_SeverityMapping" displayName="MD_SeverityMapping" ref="A59:D95" totalsRowShown="0" dataDxfId="31">
   <autoFilter ref="A59:D95" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:E61">
     <sortCondition ref="A2:A26"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Coordinates" dataDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Coordinates" dataDxfId="30">
       <calculatedColumnFormula>"i"&amp;MD_SeverityMapping[[#This Row],[Impact]]&amp;"l"&amp;MD_SeverityMapping[[#This Row],[Likelihood]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Impact" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Likelihood" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Severity" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Impact" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Likelihood" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Severity" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6211,7 +6211,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6516,6 +6516,25 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>F3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="505" id="{342793A4-491D-45A5-9776-2802D4AD1877}">
+            <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="257" id="{FFCCB9C1-BB00-48E3-A2A5-73897C425504}">
@@ -6732,25 +6751,6 @@
           </x14:cfRule>
           <xm:sqref>K3:L3</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="505" id="{342793A4-491D-45A5-9776-2802D4AD1877}">
-            <x14:iconSet iconSet="3Flags" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>G3</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -8579,7 +8579,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>